<commit_message>
Updated Sprint 1 Spreadsheet, request screenshot of output for project 3 assignment
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srikanth/Documenta/StevensInstitute/SoftwareEngg/SSW-555/Week3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06278AC2-BC39-F04E-8223-5650305B5C29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B92CB9-1406-49F1-AC95-FF446115650C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16660" tabRatio="500" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,19 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -36,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="273">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -678,6 +687,213 @@
   </si>
   <si>
     <t>Status stages : Assigned, InProgress, Done</t>
+  </si>
+  <si>
+    <t>T01.01</t>
+  </si>
+  <si>
+    <t>T01.02</t>
+  </si>
+  <si>
+    <t>T01.03</t>
+  </si>
+  <si>
+    <t>Store current date</t>
+  </si>
+  <si>
+    <t>Compare to date field</t>
+  </si>
+  <si>
+    <t>T02.01</t>
+  </si>
+  <si>
+    <t>T02.02</t>
+  </si>
+  <si>
+    <t>T02.03</t>
+  </si>
+  <si>
+    <t>Store birth date</t>
+  </si>
+  <si>
+    <t>Store marriage date</t>
+  </si>
+  <si>
+    <t>Compare birth date and marriage date</t>
+  </si>
+  <si>
+    <t>T03.01</t>
+  </si>
+  <si>
+    <t>T03.02</t>
+  </si>
+  <si>
+    <t>T03.03</t>
+  </si>
+  <si>
+    <t>Store death date</t>
+  </si>
+  <si>
+    <t>Compare birth date and death date</t>
+  </si>
+  <si>
+    <t>T04.01</t>
+  </si>
+  <si>
+    <t>T04.02</t>
+  </si>
+  <si>
+    <t>T04.03</t>
+  </si>
+  <si>
+    <t>T04.04</t>
+  </si>
+  <si>
+    <t>T02.04</t>
+  </si>
+  <si>
+    <t>Check if there was a marriage</t>
+  </si>
+  <si>
+    <t>Check if there was a divorce</t>
+  </si>
+  <si>
+    <t>Store divorce date</t>
+  </si>
+  <si>
+    <t>Compare marriage date and divorce date</t>
+  </si>
+  <si>
+    <t>T05.01</t>
+  </si>
+  <si>
+    <t>T05.02</t>
+  </si>
+  <si>
+    <t>T05.03</t>
+  </si>
+  <si>
+    <t>T05.04</t>
+  </si>
+  <si>
+    <t>T05.05</t>
+  </si>
+  <si>
+    <t>Check if there was a death</t>
+  </si>
+  <si>
+    <t>Compare marriage date and death date</t>
+  </si>
+  <si>
+    <t>T03.04</t>
+  </si>
+  <si>
+    <t>T04.05</t>
+  </si>
+  <si>
+    <t>T06.01</t>
+  </si>
+  <si>
+    <t>T06.02</t>
+  </si>
+  <si>
+    <t>T06.03</t>
+  </si>
+  <si>
+    <t>T06.04</t>
+  </si>
+  <si>
+    <t>T06.05</t>
+  </si>
+  <si>
+    <t>Compare divorce date and death date</t>
+  </si>
+  <si>
+    <t>T07.01</t>
+  </si>
+  <si>
+    <t>T07.02</t>
+  </si>
+  <si>
+    <t>T07.03</t>
+  </si>
+  <si>
+    <t>T07.04</t>
+  </si>
+  <si>
+    <t>T07.05</t>
+  </si>
+  <si>
+    <t>If death, store death date</t>
+  </si>
+  <si>
+    <t>If no death, store today's date</t>
+  </si>
+  <si>
+    <t>T07.06</t>
+  </si>
+  <si>
+    <t>Calculate age</t>
+  </si>
+  <si>
+    <t>Compare to 150 years old</t>
+  </si>
+  <si>
+    <t>T08.01</t>
+  </si>
+  <si>
+    <t>T08.02</t>
+  </si>
+  <si>
+    <t>T08.03</t>
+  </si>
+  <si>
+    <t>T09.01</t>
+  </si>
+  <si>
+    <t>T09.02</t>
+  </si>
+  <si>
+    <t>T09.03</t>
+  </si>
+  <si>
+    <t>T09.04</t>
+  </si>
+  <si>
+    <t>Store death date of parent 1</t>
+  </si>
+  <si>
+    <t>Store death date of parent 2</t>
+  </si>
+  <si>
+    <t>Compare death dates and birth date</t>
+  </si>
+  <si>
+    <t>T10.01</t>
+  </si>
+  <si>
+    <t>Check for marriage</t>
+  </si>
+  <si>
+    <t>T10.02</t>
+  </si>
+  <si>
+    <t>T10.03</t>
+  </si>
+  <si>
+    <t>T10.04</t>
+  </si>
+  <si>
+    <t>Calculate age at marriage</t>
+  </si>
+  <si>
+    <t>T10.05</t>
+  </si>
+  <si>
+    <t>Compare to 14 years old</t>
+  </si>
+  <si>
+    <t>Store date field</t>
   </si>
 </sst>
 </file>
@@ -697,26 +913,31 @@
       <b/>
       <sz val="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="10"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
       <sz val="10"/>
       <color theme="11"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -821,7 +1042,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -851,10 +1072,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="65"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -964,7 +1188,7 @@
             <c:numRef>
               <c:f>'Burndown README'!$B$15:$B$20</c:f>
               <c:numCache>
-                <c:formatCode>m/d/yy</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>42632</c:v>
@@ -1035,7 +1259,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1101,13 +1325,22 @@
             <c:numRef>
               <c:f>Burndown!$A$2:$A$7</c:f>
               <c:numCache>
-                <c:formatCode>m/d</c:formatCode>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
+                  <c:v>42632</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>42647</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>42675</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42689</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1119,7 +1352,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30</c:v>
@@ -1154,7 +1387,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="m/d" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2013,19 +2246,19 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="4" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="4" max="4" width="22.84375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -2042,7 +2275,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>180</v>
       </c>
@@ -2059,7 +2292,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>196</v>
       </c>
@@ -2076,7 +2309,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>190</v>
       </c>
@@ -2093,7 +2326,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2110,7 +2343,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>186</v>
       </c>
@@ -2127,7 +2360,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
@@ -2136,7 +2369,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D4">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D4">
     <sortCondition ref="C2:C4"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2156,20 +2389,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A29" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>29</v>
       </c>
@@ -2187,7 +2420,7 @@
       </c>
       <c r="G1" s="18"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2204,7 +2437,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2220,14 +2453,14 @@
       <c r="E3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="20" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2244,7 +2477,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2261,7 +2494,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2278,7 +2511,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2295,7 +2528,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2312,7 +2545,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2329,7 +2562,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2346,7 +2579,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2363,7 +2596,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2380,7 +2613,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2397,7 +2630,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2414,7 +2647,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2431,7 +2664,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2448,7 +2681,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2465,7 +2698,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2482,7 +2715,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2499,7 +2732,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2516,7 +2749,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>2</v>
       </c>
@@ -2533,7 +2766,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2550,7 +2783,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2567,7 +2800,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2584,7 +2817,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2601,7 +2834,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>3</v>
       </c>
@@ -2618,7 +2851,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>3</v>
       </c>
@@ -2635,7 +2868,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>3</v>
       </c>
@@ -2652,7 +2885,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>3</v>
       </c>
@@ -2669,7 +2902,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>3</v>
       </c>
@@ -2686,7 +2919,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2703,7 +2936,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2720,7 +2953,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2737,7 +2970,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>4</v>
       </c>
@@ -2754,7 +2987,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>4</v>
       </c>
@@ -2771,7 +3004,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2788,7 +3021,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>4</v>
       </c>
@@ -2805,7 +3038,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>4</v>
       </c>
@@ -2822,7 +3055,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>4</v>
       </c>
@@ -2839,7 +3072,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>4</v>
       </c>
@@ -2856,7 +3089,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>4</v>
       </c>
@@ -2887,51 +3120,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="7"/>
+    <col min="2" max="2" width="10.23046875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3046875" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>161</v>
       </c>
@@ -2954,7 +3187,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>162</v>
       </c>
@@ -2970,14 +3203,14 @@
       <c r="F15" s="14"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>163</v>
       </c>
       <c r="B16" s="13">
         <v>42647</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="19">
         <v>10</v>
       </c>
       <c r="D16">
@@ -2994,14 +3227,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="13">
         <v>42661</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="19">
         <v>10</v>
       </c>
       <c r="D17">
@@ -3019,14 +3252,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>165</v>
       </c>
       <c r="B18" s="13">
         <v>42675</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="19">
         <v>10</v>
       </c>
       <c r="D18">
@@ -3044,14 +3277,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>166</v>
       </c>
       <c r="B19" s="13">
         <v>42689</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="19">
         <v>10</v>
       </c>
       <c r="D19">
@@ -3078,23 +3311,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.1640625" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.84375" style="2"/>
+    <col min="2" max="2" width="16.69140625" customWidth="1"/>
+    <col min="3" max="3" width="12.4609375" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.4609375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3114,27 +3347,27 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="2">
-        <v>40442</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>42632</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="2">
-        <v>40455</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>42647</v>
       </c>
       <c r="B3">
         <v>30</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3">
         <v>250</v>
@@ -3145,6 +3378,21 @@
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
         <v>125.00000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>42661</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>42675</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>42689</v>
       </c>
     </row>
   </sheetData>
@@ -3157,25 +3405,25 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.07421875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.4609375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.4609375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.3046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.4609375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3046875" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3204,22 +3452,884 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14" x14ac:dyDescent="0.15">
-      <c r="B14" s="5" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I3" s="7"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="B14" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D15" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16">
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B18" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B19" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="B20" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I21" s="7"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E22">
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" s="7"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="B25" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="B27" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D27" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>119</v>
+      </c>
+      <c r="B28" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D28" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E28">
+        <v>7</v>
+      </c>
+      <c r="F28">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D29" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I29" s="7"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I30" s="7"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I31" s="7"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I32" s="7"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I33" s="7"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>120</v>
+      </c>
+      <c r="B34" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E34">
+        <v>9</v>
+      </c>
+      <c r="F34">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="B35" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D35" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I35" s="7"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D36" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I36" s="7"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I37" s="7"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I38" s="7"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>252</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I39" s="7"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="17" t="s">
+        <v>251</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I40" s="7"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>121</v>
+      </c>
+      <c r="B41" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E41">
+        <v>3</v>
+      </c>
+      <c r="F41">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A42" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="C42" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I42" s="7"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C43" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I43" s="7"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I44" s="7"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="C46" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I46" s="7"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C47" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I47" s="7"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I48" s="7"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I49" s="7"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>123</v>
+      </c>
+      <c r="B50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="E50">
+        <v>12</v>
+      </c>
+      <c r="F50">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="B51" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="C51" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A52" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="B52" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I52" s="7"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A53" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="B53" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I53" s="7"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A54" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="B54" s="21" t="s">
+        <v>269</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A55" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B55" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="C55" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="I55" s="7"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A56" s="17"/>
+      <c r="I56" s="7"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B57" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="B15" s="5"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="14" x14ac:dyDescent="0.15">
-      <c r="B16" s="5" t="s">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B58" s="5"/>
+      <c r="I58" s="7"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B59" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="14" x14ac:dyDescent="0.15">
-      <c r="B20" s="5" t="s">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B63" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3238,9 +4348,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3284,9 +4394,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3329,9 +4439,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3370,17 +4480,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="B35" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.15234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.4609375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>113</v>
       </c>
@@ -3391,7 +4501,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -3402,7 +4512,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -3413,7 +4523,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -3424,7 +4534,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -3435,7 +4545,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -3446,7 +4556,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -3457,7 +4567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -3468,7 +4578,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -3479,7 +4589,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -3490,7 +4600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -3501,7 +4611,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -3512,7 +4622,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -3523,7 +4633,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="68" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -3534,7 +4644,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -3545,7 +4655,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -3556,7 +4666,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -3567,7 +4677,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -3578,7 +4688,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -3589,7 +4699,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -3600,7 +4710,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -3611,7 +4721,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -3622,7 +4732,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -3633,7 +4743,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -3644,7 +4754,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:3" ht="45" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -3655,7 +4765,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -3666,7 +4776,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="136" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:3" ht="105" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -3677,7 +4787,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -3688,7 +4798,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -3699,7 +4809,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -3710,7 +4820,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -3721,7 +4831,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -3732,7 +4842,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="17" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:3" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -3743,7 +4853,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -3754,7 +4864,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="51" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -3765,7 +4875,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -3776,7 +4886,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -3787,7 +4897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -3798,7 +4908,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -3809,7 +4919,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -3820,7 +4930,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -3831,7 +4941,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -3842,7 +4952,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="34" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Small update to error message
</commit_message>
<xml_diff>
--- a/Team2Report.xlsx
+++ b/Team2Report.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project\Agile_Methods_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztyle\Documents\SSW 555\SSW_555_Project_Sprint1\Agile_Methods_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B92CB9-1406-49F1-AC95-FF446115650C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555EC9FA-12D8-4BF8-8FA8-3A8377A31FF9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="274">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -894,6 +894,9 @@
   </si>
   <si>
     <t>Store date field</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -1073,11 +1076,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="66">
@@ -2453,12 +2456,12 @@
       <c r="E3" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="21" t="s">
         <v>203</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3120,7 +3123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="150" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3407,8 +3410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
@@ -3491,7 +3494,7 @@
       <c r="A4" s="17" t="s">
         <v>205</v>
       </c>
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>272</v>
       </c>
       <c r="C4" s="17" t="s">
@@ -4228,41 +4231,50 @@
         <v>186</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
       <c r="E50">
         <v>12</v>
       </c>
       <c r="F50">
         <v>240</v>
+      </c>
+      <c r="G50">
+        <v>14</v>
+      </c>
+      <c r="H50">
+        <v>60</v>
+      </c>
+      <c r="I50" s="6">
+        <v>42636</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="17" t="s">
         <v>264</v>
       </c>
-      <c r="B51" s="21" t="s">
+      <c r="B51" s="20" t="s">
         <v>265</v>
       </c>
       <c r="C51" s="17" t="s">
         <v>186</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="17" t="s">
         <v>266</v>
       </c>
-      <c r="B52" s="21" t="s">
+      <c r="B52" s="20" t="s">
         <v>213</v>
       </c>
       <c r="C52" s="17" t="s">
         <v>186</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
       <c r="I52" s="7"/>
     </row>
@@ -4270,14 +4282,14 @@
       <c r="A53" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="B53" s="21" t="s">
+      <c r="B53" s="20" t="s">
         <v>212</v>
       </c>
       <c r="C53" s="17" t="s">
         <v>186</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
       <c r="I53" s="7"/>
     </row>
@@ -4285,28 +4297,28 @@
       <c r="A54" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="B54" s="21" t="s">
+      <c r="B54" s="20" t="s">
         <v>269</v>
       </c>
       <c r="C54" s="17" t="s">
         <v>186</v>
       </c>
       <c r="D54" s="17" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="B55" s="20" t="s">
         <v>271</v>
       </c>
       <c r="C55" s="17" t="s">
         <v>186</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>202</v>
+        <v>273</v>
       </c>
       <c r="I55" s="7"/>
     </row>
@@ -4710,7 +4722,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>133</v>
       </c>

</xml_diff>